<commit_message>
23.09.07 add: update compatibility
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="72">
   <si>
     <t>序号</t>
   </si>
@@ -210,6 +210,47 @@
   </si>
   <si>
     <t>exp53</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>train: [/workspace/dataset/VisDrone/VisDrone2019-DET-train/JPEGImages,
+        ]</t>
+  </si>
+  <si>
+    <t>test:  [
+/workspace/dataset/VisDrone/VisDrone2019-DET-test-dev/JPEGImages,
+]</t>
+  </si>
+  <si>
+    <t>exp63</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>train: [
+        /workspace/dataset/VisDrone/VisDrone2019-DET-train/JPEGImages,
+        /workspace/dataset/VisDrone/VisDrone2019-DET-val/JPEGImages,
+        /workspace/dataset/VisDrone/VisDrone2019-DET-test-dev/JPEGImages,
+        /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/train/baoan_2d_220801_sub1/VOC2007/JPEGImages,
+        /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/train/VOCdevkitszcity1_specialcar_sub1/VOC2007/JPEGImages,
+        /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/train/voc_2007_2012_Pedestrain/VOCdevkit/VOC2007/JPEGImages,
+        /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/train/voc_2007_2012_Pedestrain/VOCdevkit/VOC2012/JPEGImages,        
+]</t>
+  </si>
+  <si>
+    <t>test:  [
+  /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/val/baoan_2d_220801_sub2/VOC2007/JPEGImages,
+  /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/val/baoan_jiaolian/VOC2007/JPEGImages,
+  /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/val/futian_special/VOC2007/JPEGImages,
+  /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/val/task_baoan-2021_09_27_13_45_46/VOC2007/JPEGImages,
+  /workspace/dataset/sutpc_object_detections_datasets_vehicle_count/val/VOCdevkitszcity1_specialcar_sub2/VOC2007/JPEGImages,
+]</t>
+  </si>
+  <si>
+    <t>exp70</t>
   </si>
   <si>
     <t xml:space="preserve">["Car", 
@@ -238,39 +279,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,7 +295,99 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,14 +408,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -328,59 +422,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -391,13 +432,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,37 +576,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,127 +612,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,11 +641,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,6 +667,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -656,30 +721,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -692,8 +733,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -702,152 +743,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -862,6 +903,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1889,8 +1933,8 @@
   <sheetPr/>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15"/>
@@ -2013,6 +2057,34 @@
         <v>62</v>
       </c>
     </row>
+    <row r="4" spans="2:13">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="17" ht="15.75" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>0</v>
@@ -2104,7 +2176,7 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>